<commit_message>
Timer and testing updates
Created Timer manager and timer main class. Updated text handler test to
test all PWS inputs. Began updates to DTP to test for timer
functionality.
</commit_message>
<xml_diff>
--- a/Documents/Software/Testing and Integration/eCook's DTP Record - 4th Iteration layering integration.xlsx
+++ b/Documents/Software/Testing and Integration/eCook's DTP Record - 4th Iteration layering integration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20490" windowHeight="7635" tabRatio="757" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20490" windowHeight="7635" tabRatio="757" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="DTP" sheetId="10" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Display Text on Slide" sheetId="13" r:id="rId6"/>
     <sheet name="Display Image on Slide" sheetId="14" r:id="rId7"/>
     <sheet name="Move Between Slides" sheetId="15" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="97">
   <si>
     <t>Expected Outcome</t>
   </si>
@@ -1161,6 +1162,12 @@
   </si>
   <si>
     <t>Layering now implemented and successful.</t>
+  </si>
+  <si>
+    <t>Start and Use timer Feature (Timer)</t>
+  </si>
+  <si>
+    <t>In the slideshow class, configure the XML parser URL to an XML playlist within the Resources folder</t>
   </si>
 </sst>
 </file>
@@ -1581,7 +1588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5040,8 +5047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5713,4 +5720,105 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21">
+      <c r="A1" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>